<commit_message>
finish fixing the peaks identifying and filling pipelines
</commit_message>
<xml_diff>
--- a/Best ch pipeline/improved_best_channels_stat.xlsx
+++ b/Best ch pipeline/improved_best_channels_stat.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Mom_9m_Toys" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Infant_9m_NoToys" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Mom_9m_NoToys" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="excluded subs" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -459,27 +460,27 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>length_ibis_ts_best</t>
+          <t>length_ibis_ts</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>long_ibi_count_best</t>
+          <t>long_ibi_count</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sdrr_best</t>
+          <t>sdrr</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mean_best</t>
+          <t>mean</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>median_best</t>
+          <t>median</t>
         </is>
       </c>
     </row>
@@ -666,19 +667,19 @@
         <v>126453</v>
       </c>
       <c r="E7" t="n">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>46.09057467912736</v>
+        <v>46.90922428222573</v>
       </c>
       <c r="H7" t="n">
-        <v>209.2255389718076</v>
+        <v>210.2716666666667</v>
       </c>
       <c r="I7" t="n">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8">
@@ -930,16 +931,16 @@
         <v>98547</v>
       </c>
       <c r="E15" t="n">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>58.68016482928107</v>
+        <v>58.9875155194828</v>
       </c>
       <c r="H15" t="n">
-        <v>209.6844349680171</v>
+        <v>210.5824411134904</v>
       </c>
       <c r="I15" t="n">
         <v>202</v>
@@ -963,16 +964,16 @@
         <v>149857</v>
       </c>
       <c r="E16" t="n">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>29.17218674398293</v>
+        <v>29.64543133834556</v>
       </c>
       <c r="H16" t="n">
-        <v>216.0722543352601</v>
+        <v>216.3849493487699</v>
       </c>
       <c r="I16" t="n">
         <v>212</v>
@@ -1128,16 +1129,16 @@
         <v>150130</v>
       </c>
       <c r="E21" t="n">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>16.38226233726212</v>
+        <v>17.20647010474488</v>
       </c>
       <c r="H21" t="n">
-        <v>208.7242339832869</v>
+        <v>209.0153417015342</v>
       </c>
       <c r="I21" t="n">
         <v>208</v>
@@ -1161,16 +1162,16 @@
         <v>150121</v>
       </c>
       <c r="E22" t="n">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F22" t="n">
         <v>7</v>
       </c>
       <c r="G22" t="n">
-        <v>51.04885176948098</v>
+        <v>51.83226834444993</v>
       </c>
       <c r="H22" t="n">
-        <v>230.9075500770416</v>
+        <v>231.2638888888889</v>
       </c>
       <c r="I22" t="n">
         <v>226</v>
@@ -1227,16 +1228,16 @@
         <v>150100</v>
       </c>
       <c r="E24" t="n">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F24" t="n">
         <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>21.93215345829074</v>
+        <v>22.72627787155751</v>
       </c>
       <c r="H24" t="n">
-        <v>221.3190546528804</v>
+        <v>221.646449704142</v>
       </c>
       <c r="I24" t="n">
         <v>221</v>
@@ -1431,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>19.67961638491253</v>
+        <v>19.64777886291388</v>
       </c>
       <c r="H30" t="n">
         <v>249.3533333333333</v>
@@ -1656,19 +1657,19 @@
         <v>147583</v>
       </c>
       <c r="E37" t="n">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F37" t="n">
         <v>56</v>
       </c>
       <c r="G37" t="n">
-        <v>1162.437850352354</v>
+        <v>1168.369872788458</v>
       </c>
       <c r="H37" t="n">
-        <v>713.1213592233009</v>
+        <v>720.1127450980392</v>
       </c>
       <c r="I37" t="n">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38">
@@ -1689,16 +1690,16 @@
         <v>150146</v>
       </c>
       <c r="E38" t="n">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F38" t="n">
         <v>7</v>
       </c>
       <c r="G38" t="n">
-        <v>153.2618598096926</v>
+        <v>154.3570465411999</v>
       </c>
       <c r="H38" t="n">
-        <v>236.6919431279621</v>
+        <v>238.5764331210191</v>
       </c>
       <c r="I38" t="n">
         <v>212</v>
@@ -1943,14 +1944,14 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ch_0</t>
+          <t>ch_1</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>149.639</v>
+        <v>149.658</v>
       </c>
       <c r="D46" t="n">
-        <v>149639</v>
+        <v>149658</v>
       </c>
       <c r="E46" t="n">
         <v>669</v>
@@ -1959,10 +1960,10 @@
         <v>4</v>
       </c>
       <c r="G46" t="n">
-        <v>40.16110700987912</v>
+        <v>38.2053742037219</v>
       </c>
       <c r="H46" t="n">
-        <v>223.2869955156951</v>
+        <v>223.3243647234679</v>
       </c>
       <c r="I46" t="n">
         <v>220</v>
@@ -2283,16 +2284,16 @@
         <v>150333</v>
       </c>
       <c r="E56" t="n">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F56" t="n">
         <v>4</v>
       </c>
       <c r="G56" t="n">
-        <v>855.1023165926097</v>
+        <v>855.9063164464903</v>
       </c>
       <c r="H56" t="n">
-        <v>254.8539898132428</v>
+        <v>255.2874149659864</v>
       </c>
       <c r="I56" t="n">
         <v>212</v>
@@ -2316,16 +2317,16 @@
         <v>149964</v>
       </c>
       <c r="E57" t="n">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="F57" t="n">
         <v>1</v>
       </c>
       <c r="G57" t="n">
-        <v>31.15268159137176</v>
+        <v>33.65055211301559</v>
       </c>
       <c r="H57" t="n">
-        <v>210.5147679324895</v>
+        <v>211.1086036671368</v>
       </c>
       <c r="I57" t="n">
         <v>208</v>
@@ -2349,19 +2350,19 @@
         <v>150089</v>
       </c>
       <c r="E58" t="n">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="F58" t="n">
         <v>3</v>
       </c>
       <c r="G58" t="n">
-        <v>66.47786140078594</v>
+        <v>68.51502869115996</v>
       </c>
       <c r="H58" t="n">
-        <v>225.894419306184</v>
+        <v>227.9573820395738</v>
       </c>
       <c r="I58" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59">
@@ -2646,19 +2647,19 @@
         <v>59893</v>
       </c>
       <c r="E67" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F67" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G67" t="n">
-        <v>468.325977269427</v>
+        <v>469.3268835771313</v>
       </c>
       <c r="H67" t="n">
-        <v>587.3232323232323</v>
+        <v>593.3163265306123</v>
       </c>
       <c r="I67" t="n">
-        <v>373</v>
+        <v>391</v>
       </c>
     </row>
     <row r="68">
@@ -2967,27 +2968,27 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>length_ibis_ts_best</t>
+          <t>length_ibis_ts</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>long_ibi_count_best</t>
+          <t>long_ibi_count</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sdrr_best</t>
+          <t>sdrr</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mean_best</t>
+          <t>mean</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>median_best</t>
+          <t>median</t>
         </is>
       </c>
     </row>
@@ -3108,16 +3109,16 @@
         <v>149870</v>
       </c>
       <c r="E5" t="n">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>34.47991949209992</v>
+        <v>36.26321325436572</v>
       </c>
       <c r="H5" t="n">
-        <v>344.4930875576037</v>
+        <v>345.2886836027714</v>
       </c>
       <c r="I5" t="n">
         <v>345</v>
@@ -3339,19 +3340,19 @@
         <v>149990</v>
       </c>
       <c r="E12" t="n">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F12" t="n">
         <v>3</v>
       </c>
       <c r="G12" t="n">
-        <v>81.39856785452363</v>
+        <v>82.00392047790697</v>
       </c>
       <c r="H12" t="n">
-        <v>314.9684210526316</v>
+        <v>315.632911392405</v>
       </c>
       <c r="I12" t="n">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13">
@@ -3405,19 +3406,19 @@
         <v>149498</v>
       </c>
       <c r="E14" t="n">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F14" t="n">
         <v>4</v>
       </c>
       <c r="G14" t="n">
-        <v>160.6564431564435</v>
+        <v>161.95345404552</v>
       </c>
       <c r="H14" t="n">
-        <v>454.3780487804878</v>
+        <v>455.7675840978594</v>
       </c>
       <c r="I14" t="n">
-        <v>484.5</v>
+        <v>485</v>
       </c>
     </row>
     <row r="15">
@@ -3444,7 +3445,7 @@
         <v>7</v>
       </c>
       <c r="G15" t="n">
-        <v>234.4868139647853</v>
+        <v>234.4780014841328</v>
       </c>
       <c r="H15" t="n">
         <v>430.4096916299559</v>
@@ -3537,19 +3538,19 @@
         <v>75010</v>
       </c>
       <c r="E18" t="n">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>55.56137962654655</v>
+        <v>58.00626898111504</v>
       </c>
       <c r="H18" t="n">
-        <v>194.84375</v>
+        <v>201.1290322580645</v>
       </c>
       <c r="I18" t="n">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
@@ -3570,19 +3571,19 @@
         <v>149990</v>
       </c>
       <c r="E19" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F19" t="n">
         <v>24</v>
       </c>
       <c r="G19" t="n">
-        <v>1131.571740219993</v>
+        <v>1134.837767372045</v>
       </c>
       <c r="H19" t="n">
-        <v>659.6106194690266</v>
+        <v>662.5422222222222</v>
       </c>
       <c r="I19" t="n">
-        <v>419.5</v>
+        <v>420</v>
       </c>
     </row>
     <row r="20">
@@ -3636,19 +3637,19 @@
         <v>149776</v>
       </c>
       <c r="E21" t="n">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>96.11030029704173</v>
+        <v>98.47807930701568</v>
       </c>
       <c r="H21" t="n">
-        <v>441.905325443787</v>
+        <v>443.2166172106825</v>
       </c>
       <c r="I21" t="n">
-        <v>458.5</v>
+        <v>459</v>
       </c>
     </row>
     <row r="22">
@@ -3702,16 +3703,16 @@
         <v>150000</v>
       </c>
       <c r="E23" t="n">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>96.09613997038062</v>
+        <v>96.67824306277116</v>
       </c>
       <c r="H23" t="n">
-        <v>373.2219451371571</v>
+        <v>374.155</v>
       </c>
       <c r="I23" t="n">
         <v>370</v>
@@ -3999,16 +4000,16 @@
         <v>145785</v>
       </c>
       <c r="E32" t="n">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>46.63594629229976</v>
+        <v>48.32103884563151</v>
       </c>
       <c r="H32" t="n">
-        <v>332.2009132420091</v>
+        <v>332.9610983981693</v>
       </c>
       <c r="I32" t="n">
         <v>328</v>
@@ -4230,16 +4231,16 @@
         <v>148993</v>
       </c>
       <c r="E39" t="n">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F39" t="n">
         <v>16</v>
       </c>
       <c r="G39" t="n">
-        <v>909.6552343541438</v>
+        <v>912.5951564368033</v>
       </c>
       <c r="H39" t="n">
-        <v>474.8338658146965</v>
+        <v>477.887459807074</v>
       </c>
       <c r="I39" t="n">
         <v>336</v>
@@ -4329,16 +4330,16 @@
         <v>149876</v>
       </c>
       <c r="E42" t="n">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="F42" t="n">
         <v>2</v>
       </c>
       <c r="G42" t="n">
-        <v>92.28358204299994</v>
+        <v>96.50601092835234</v>
       </c>
       <c r="H42" t="n">
-        <v>368.2758620689655</v>
+        <v>371.0173697270471</v>
       </c>
       <c r="I42" t="n">
         <v>357</v>
@@ -5088,16 +5089,16 @@
         <v>150185</v>
       </c>
       <c r="E65" t="n">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F65" t="n">
         <v>6</v>
       </c>
       <c r="G65" t="n">
-        <v>159.5988846618943</v>
+        <v>160.9776735948541</v>
       </c>
       <c r="H65" t="n">
-        <v>424.8810198300283</v>
+        <v>427.3019943019943</v>
       </c>
       <c r="I65" t="n">
         <v>407</v>
@@ -5319,19 +5320,19 @@
         <v>110273</v>
       </c>
       <c r="E72" t="n">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F72" t="n">
         <v>2</v>
       </c>
       <c r="G72" t="n">
-        <v>165.1955991457803</v>
+        <v>167.9486380349468</v>
       </c>
       <c r="H72" t="n">
-        <v>389.1914893617021</v>
+        <v>390.576512455516</v>
       </c>
       <c r="I72" t="n">
-        <v>379.5</v>
+        <v>380</v>
       </c>
     </row>
     <row r="73">
@@ -5418,19 +5419,19 @@
         <v>103611</v>
       </c>
       <c r="E75" t="n">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F75" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G75" t="n">
-        <v>467.7467735237224</v>
+        <v>473.0011999058121</v>
       </c>
       <c r="H75" t="n">
-        <v>623.7317073170732</v>
+        <v>631.4320987654321</v>
       </c>
       <c r="I75" t="n">
-        <v>453.5</v>
+        <v>461</v>
       </c>
     </row>
     <row r="76">
@@ -5451,19 +5452,19 @@
         <v>150426</v>
       </c>
       <c r="E76" t="n">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F76" t="n">
         <v>1</v>
       </c>
       <c r="G76" t="n">
-        <v>98.91918703225727</v>
+        <v>105.553114007537</v>
       </c>
       <c r="H76" t="n">
-        <v>414.267955801105</v>
+        <v>418.8966480446927</v>
       </c>
       <c r="I76" t="n">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="77">
@@ -5484,16 +5485,16 @@
         <v>104019</v>
       </c>
       <c r="E77" t="n">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>70.52848124457712</v>
+        <v>74.95907155897538</v>
       </c>
       <c r="H77" t="n">
-        <v>322.6666666666667</v>
+        <v>325.7106918238994</v>
       </c>
       <c r="I77" t="n">
         <v>305</v>
@@ -5607,27 +5608,27 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>length_ibis_ts_best</t>
+          <t>length_ibis_ts</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>long_ibi_count_best</t>
+          <t>long_ibi_count</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sdrr_best</t>
+          <t>sdrr</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mean_best</t>
+          <t>mean</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>median_best</t>
+          <t>median</t>
         </is>
       </c>
     </row>
@@ -6177,16 +6178,16 @@
         <v>36643</v>
       </c>
       <c r="E18" t="n">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>65.59075431966045</v>
+        <v>66.28927834758096</v>
       </c>
       <c r="H18" t="n">
-        <v>222.4207317073171</v>
+        <v>223.7852760736196</v>
       </c>
       <c r="I18" t="n">
         <v>211</v>
@@ -6276,19 +6277,19 @@
         <v>75011</v>
       </c>
       <c r="E21" t="n">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>49.46337739730133</v>
+        <v>53.44561693295265</v>
       </c>
       <c r="H21" t="n">
-        <v>223.6826347305389</v>
+        <v>228.4709480122324</v>
       </c>
       <c r="I21" t="n">
-        <v>216.5</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22">
@@ -6375,19 +6376,19 @@
         <v>74948</v>
       </c>
       <c r="E24" t="n">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F24" t="n">
         <v>7</v>
       </c>
       <c r="G24" t="n">
-        <v>109.2355524402559</v>
+        <v>111.0912143300063</v>
       </c>
       <c r="H24" t="n">
-        <v>233.38125</v>
+        <v>234.8490566037736</v>
       </c>
       <c r="I24" t="n">
-        <v>208.5</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25">
@@ -6728,7 +6729,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ch_2</t>
+          <t>ch_0</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -6738,19 +6739,19 @@
         <v>74497</v>
       </c>
       <c r="E35" t="n">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F35" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G35" t="n">
-        <v>1330.320776972866</v>
+        <v>1292.239490429687</v>
       </c>
       <c r="H35" t="n">
-        <v>1196.677419354839</v>
+        <v>1030.472222222222</v>
       </c>
       <c r="I35" t="n">
-        <v>783.5</v>
+        <v>570.5</v>
       </c>
     </row>
     <row r="36">
@@ -6936,19 +6937,19 @@
         <v>74935</v>
       </c>
       <c r="E41" t="n">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>45.64032132628125</v>
+        <v>47.50909961870469</v>
       </c>
       <c r="H41" t="n">
-        <v>205.2912087912088</v>
+        <v>207.5722222222222</v>
       </c>
       <c r="I41" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42">
@@ -7299,19 +7300,19 @@
         <v>68743</v>
       </c>
       <c r="E52" t="n">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>31.40815434133996</v>
+        <v>32.00838002774287</v>
       </c>
       <c r="H52" t="n">
-        <v>199.0552325581395</v>
+        <v>199.6355685131195</v>
       </c>
       <c r="I52" t="n">
-        <v>198.5</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53">
@@ -7322,14 +7323,14 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ch_0</t>
+          <t>ch_2</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>74.93899999999999</v>
+        <v>74.937</v>
       </c>
       <c r="D53" t="n">
-        <v>74939</v>
+        <v>74937</v>
       </c>
       <c r="E53" t="n">
         <v>368</v>
@@ -7338,7 +7339,7 @@
         <v>7</v>
       </c>
       <c r="G53" t="n">
-        <v>108.062973206265</v>
+        <v>107.8566192677451</v>
       </c>
       <c r="H53" t="n">
         <v>202.7880434782609</v>
@@ -7398,16 +7399,16 @@
         <v>75051</v>
       </c>
       <c r="E55" t="n">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>31.6700644645867</v>
+        <v>35.66775881927214</v>
       </c>
       <c r="H55" t="n">
-        <v>220.4424778761062</v>
+        <v>222.4107142857143</v>
       </c>
       <c r="I55" t="n">
         <v>215</v>
@@ -7431,16 +7432,16 @@
         <v>75110</v>
       </c>
       <c r="E56" t="n">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F56" t="n">
         <v>6</v>
       </c>
       <c r="G56" t="n">
-        <v>90.36038888389031</v>
+        <v>90.59216429019995</v>
       </c>
       <c r="H56" t="n">
-        <v>219.5982404692082</v>
+        <v>220.2441176470588</v>
       </c>
       <c r="I56" t="n">
         <v>201</v>
@@ -7596,16 +7597,16 @@
         <v>93277</v>
       </c>
       <c r="E61" t="n">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F61" t="n">
         <v>3</v>
       </c>
       <c r="G61" t="n">
-        <v>65.11735265673258</v>
+        <v>65.68057928751597</v>
       </c>
       <c r="H61" t="n">
-        <v>247.6702127659574</v>
+        <v>248.3306666666667</v>
       </c>
       <c r="I61" t="n">
         <v>241</v>
@@ -7662,19 +7663,19 @@
         <v>22914</v>
       </c>
       <c r="E63" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F63" t="n">
         <v>1</v>
       </c>
       <c r="G63" t="n">
-        <v>76.57870085351469</v>
+        <v>78.72063262231548</v>
       </c>
       <c r="H63" t="n">
-        <v>238.021052631579</v>
+        <v>240.5531914893617</v>
       </c>
       <c r="I63" t="n">
-        <v>216</v>
+        <v>216.5</v>
       </c>
     </row>
     <row r="64">
@@ -7695,19 +7696,19 @@
         <v>74737</v>
       </c>
       <c r="E64" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F64" t="n">
         <v>31</v>
       </c>
       <c r="G64" t="n">
-        <v>1450.338686271281</v>
+        <v>1464.115850948961</v>
       </c>
       <c r="H64" t="n">
-        <v>1129.818181818182</v>
+        <v>1147.2</v>
       </c>
       <c r="I64" t="n">
-        <v>545</v>
+        <v>569</v>
       </c>
     </row>
     <row r="65">
@@ -7728,19 +7729,19 @@
         <v>60596</v>
       </c>
       <c r="E65" t="n">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F65" t="n">
         <v>25</v>
       </c>
       <c r="G65" t="n">
-        <v>354.7627251952813</v>
+        <v>355.5493699108007</v>
       </c>
       <c r="H65" t="n">
-        <v>435.3405797101449</v>
+        <v>438.5182481751825</v>
       </c>
       <c r="I65" t="n">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66">
@@ -7794,16 +7795,16 @@
         <v>49275</v>
       </c>
       <c r="E67" t="n">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F67" t="n">
         <v>1</v>
       </c>
       <c r="G67" t="n">
-        <v>870.5482249628097</v>
+        <v>872.8591110642532</v>
       </c>
       <c r="H67" t="n">
-        <v>264.6324324324324</v>
+        <v>266.0706521739131</v>
       </c>
       <c r="I67" t="n">
         <v>188</v>
@@ -7992,19 +7993,19 @@
         <v>74777</v>
       </c>
       <c r="E73" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F73" t="n">
         <v>43</v>
       </c>
       <c r="G73" t="n">
-        <v>669.4181489785126</v>
+        <v>675.076357179755</v>
       </c>
       <c r="H73" t="n">
-        <v>724.22</v>
+        <v>731.5353535353536</v>
       </c>
       <c r="I73" t="n">
-        <v>530.5</v>
+        <v>546</v>
       </c>
     </row>
     <row r="74">
@@ -8115,27 +8116,27 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>length_ibis_ts_best</t>
+          <t>length_ibis_ts</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>long_ibi_count_best</t>
+          <t>long_ibi_count</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sdrr_best</t>
+          <t>sdrr</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mean_best</t>
+          <t>mean</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>median_best</t>
+          <t>median</t>
         </is>
       </c>
     </row>
@@ -8190,16 +8191,16 @@
         <v>71763</v>
       </c>
       <c r="E3" t="n">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F3" t="n">
         <v>5</v>
       </c>
       <c r="G3" t="n">
-        <v>239.6418690057398</v>
+        <v>240.8748421789677</v>
       </c>
       <c r="H3" t="n">
-        <v>428.4550898203593</v>
+        <v>431.0361445783133</v>
       </c>
       <c r="I3" t="n">
         <v>368</v>
@@ -8487,16 +8488,16 @@
         <v>74988</v>
       </c>
       <c r="E12" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>52.27898191110526</v>
+        <v>52.91597278042619</v>
       </c>
       <c r="H12" t="n">
-        <v>296.1984126984127</v>
+        <v>297.3784860557769</v>
       </c>
       <c r="I12" t="n">
         <v>283</v>
@@ -8553,19 +8554,19 @@
         <v>75456</v>
       </c>
       <c r="E14" t="n">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F14" t="n">
         <v>4</v>
       </c>
       <c r="G14" t="n">
-        <v>208.7419307007862</v>
+        <v>210.7842003443518</v>
       </c>
       <c r="H14" t="n">
-        <v>409.1739130434783</v>
+        <v>413.6703296703297</v>
       </c>
       <c r="I14" t="n">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15">
@@ -8586,19 +8587,19 @@
         <v>74845</v>
       </c>
       <c r="E15" t="n">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F15" t="n">
         <v>14</v>
       </c>
       <c r="G15" t="n">
-        <v>439.785229739328</v>
+        <v>441.7631116430056</v>
       </c>
       <c r="H15" t="n">
-        <v>525.9084507042254</v>
+        <v>529.6382978723404</v>
       </c>
       <c r="I15" t="n">
-        <v>352.5</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16">
@@ -8718,19 +8719,19 @@
         <v>37287</v>
       </c>
       <c r="E19" t="n">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>52.93163168898709</v>
+        <v>54.42507140822192</v>
       </c>
       <c r="H19" t="n">
-        <v>198.4010695187166</v>
+        <v>204.9779005524862</v>
       </c>
       <c r="I19" t="n">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20">
@@ -8916,16 +8917,16 @@
         <v>74805</v>
       </c>
       <c r="E25" t="n">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F25" t="n">
         <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>120.2481859746229</v>
+        <v>122.7639736766612</v>
       </c>
       <c r="H25" t="n">
-        <v>378.2690355329949</v>
+        <v>382.1487179487179</v>
       </c>
       <c r="I25" t="n">
         <v>356</v>
@@ -9345,19 +9346,19 @@
         <v>75112</v>
       </c>
       <c r="E38" t="n">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F38" t="n">
         <v>7</v>
       </c>
       <c r="G38" t="n">
-        <v>296.2730988060292</v>
+        <v>300.588495456747</v>
       </c>
       <c r="H38" t="n">
-        <v>453.6969696969697</v>
+        <v>462.0987654320988</v>
       </c>
       <c r="I38" t="n">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="39">
@@ -9411,16 +9412,16 @@
         <v>74956</v>
       </c>
       <c r="E40" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F40" t="n">
         <v>2</v>
       </c>
       <c r="G40" t="n">
-        <v>103.574043859358</v>
+        <v>104.141837793851</v>
       </c>
       <c r="H40" t="n">
-        <v>271.1745454545455</v>
+        <v>272.1642335766423</v>
       </c>
       <c r="I40" t="n">
         <v>256</v>
@@ -10011,10 +10012,10 @@
         <v>1</v>
       </c>
       <c r="G58" t="n">
-        <v>136.2685317391001</v>
+        <v>136.2567383249071</v>
       </c>
       <c r="H58" t="n">
-        <v>323.4112554112554</v>
+        <v>323.4329004329005</v>
       </c>
       <c r="I58" t="n">
         <v>311</v>
@@ -10071,16 +10072,16 @@
         <v>61086</v>
       </c>
       <c r="E60" t="n">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F60" t="n">
         <v>1</v>
       </c>
       <c r="G60" t="n">
-        <v>129.5063799162975</v>
+        <v>131.3086737097403</v>
       </c>
       <c r="H60" t="n">
-        <v>369</v>
+        <v>371.25</v>
       </c>
       <c r="I60" t="n">
         <v>329</v>
@@ -10368,19 +10369,19 @@
         <v>54225</v>
       </c>
       <c r="E69" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F69" t="n">
         <v>10</v>
       </c>
       <c r="G69" t="n">
-        <v>759.0883272115914</v>
+        <v>773.101480867737</v>
       </c>
       <c r="H69" t="n">
-        <v>627.6860465116279</v>
+        <v>635.0705882352942</v>
       </c>
       <c r="I69" t="n">
-        <v>396.5</v>
+        <v>397</v>
       </c>
     </row>
     <row r="70">
@@ -10401,16 +10402,16 @@
         <v>41858</v>
       </c>
       <c r="E70" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>73.74392923720795</v>
+        <v>78.05300140313237</v>
       </c>
       <c r="H70" t="n">
-        <v>383.8981481481482</v>
+        <v>387.4859813084112</v>
       </c>
       <c r="I70" t="n">
         <v>380</v>
@@ -10500,19 +10501,19 @@
         <v>52248</v>
       </c>
       <c r="E73" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F73" t="n">
         <v>12</v>
       </c>
       <c r="G73" t="n">
-        <v>617.7871826822078</v>
+        <v>620.8152448162034</v>
       </c>
       <c r="H73" t="n">
-        <v>637.4938271604939</v>
+        <v>645.4625</v>
       </c>
       <c r="I73" t="n">
-        <v>417</v>
+        <v>437.5</v>
       </c>
     </row>
     <row r="74">
@@ -10678,6 +10679,267 @@
       </c>
       <c r="I78" t="n">
         <v>407</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>sub_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>reason</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>participant</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>group</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_0 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>infant</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_0 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>infant</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_0 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>infant</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>82</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_2 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>infant</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_1 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_1 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>infant</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>no_toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_2 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>infant</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>no_toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_2 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>infant</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>no_toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_2 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>infant</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>no_toys</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>IBI data for best channel ch_2 does not match peak differences</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>mom</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>no_toys</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>